<commit_message>
update status for Module schedule
</commit_message>
<xml_diff>
--- a/References/Modules.xlsx
+++ b/References/Modules.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21001"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0E2CF9A2-EF86-410A-9C2F-3970662A0E50}" xr6:coauthVersionLast="38" xr6:coauthVersionMax="38" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DBC5CD49-8A72-48A9-9B8E-44E137C7FF80}" xr6:coauthVersionLast="38" xr6:coauthVersionMax="38" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="114" uniqueCount="76">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="575" uniqueCount="77">
   <si>
     <t>Hardware</t>
   </si>
@@ -263,6 +263,9 @@
   </si>
   <si>
     <t>Chưa đổ lên board test</t>
+  </si>
+  <si>
+    <t>thiếu bên slave</t>
   </si>
 </sst>
 </file>
@@ -293,7 +296,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="9">
+  <fills count="10">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -342,6 +345,12 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFF0000"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="19">
     <border>
@@ -604,7 +613,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="9" fontId="2" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="44">
+  <cellXfs count="46">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -693,41 +702,47 @@
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="1" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="9" fontId="0" fillId="0" borderId="1" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="8" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="8" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="14" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="14" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -1017,8 +1032,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="B1:J27"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B10" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="H15" sqref="H15"/>
+    <sheetView tabSelected="1" topLeftCell="B4" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="J6" sqref="J6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1065,10 +1080,10 @@
       </c>
     </row>
     <row r="3" spans="2:10" ht="90" x14ac:dyDescent="0.25">
-      <c r="B3" s="35" t="s">
+      <c r="B3" s="42" t="s">
         <v>0</v>
       </c>
-      <c r="C3" s="32" t="s">
+      <c r="C3" s="43" t="s">
         <v>7</v>
       </c>
       <c r="D3" s="6" t="s">
@@ -1082,14 +1097,14 @@
         <v>1</v>
       </c>
       <c r="H3" s="20"/>
-      <c r="I3" s="40" t="s">
+      <c r="I3" s="32" t="s">
         <v>59</v>
       </c>
       <c r="J3" s="25"/>
     </row>
     <row r="4" spans="2:10" ht="30" x14ac:dyDescent="0.25">
-      <c r="B4" s="34"/>
-      <c r="C4" s="33"/>
+      <c r="B4" s="36"/>
+      <c r="C4" s="38"/>
       <c r="D4" s="3" t="s">
         <v>2</v>
       </c>
@@ -1101,7 +1116,7 @@
         <v>1</v>
       </c>
       <c r="H4" s="16"/>
-      <c r="I4" s="40" t="s">
+      <c r="I4" s="32" t="s">
         <v>59</v>
       </c>
       <c r="J4" s="26" t="s">
@@ -1109,8 +1124,8 @@
       </c>
     </row>
     <row r="5" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B5" s="34"/>
-      <c r="C5" s="33" t="s">
+      <c r="B5" s="36"/>
+      <c r="C5" s="38" t="s">
         <v>3</v>
       </c>
       <c r="D5" s="3" t="s">
@@ -1132,8 +1147,8 @@
       </c>
     </row>
     <row r="6" spans="2:10" ht="30" x14ac:dyDescent="0.25">
-      <c r="B6" s="34"/>
-      <c r="C6" s="33"/>
+      <c r="B6" s="36"/>
+      <c r="C6" s="38"/>
       <c r="D6" s="3" t="s">
         <v>8</v>
       </c>
@@ -1150,13 +1165,13 @@
       <c r="I6" s="28" t="s">
         <v>58</v>
       </c>
-      <c r="J6" s="26" t="s">
+      <c r="J6" s="45" t="s">
         <v>73</v>
       </c>
     </row>
     <row r="7" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B7" s="34"/>
-      <c r="C7" s="33"/>
+      <c r="B7" s="36"/>
+      <c r="C7" s="38"/>
       <c r="D7" s="3" t="s">
         <v>41</v>
       </c>
@@ -1170,7 +1185,7 @@
         <v>1</v>
       </c>
       <c r="H7" s="16"/>
-      <c r="I7" s="40" t="s">
+      <c r="I7" s="32" t="s">
         <v>59</v>
       </c>
       <c r="J7" s="26" t="s">
@@ -1178,10 +1193,10 @@
       </c>
     </row>
     <row r="8" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B8" s="38" t="s">
+      <c r="B8" s="40" t="s">
         <v>36</v>
       </c>
-      <c r="C8" s="33" t="s">
+      <c r="C8" s="38" t="s">
         <v>3</v>
       </c>
       <c r="D8" s="3" t="s">
@@ -1207,8 +1222,8 @@
       </c>
     </row>
     <row r="9" spans="2:10" ht="30" x14ac:dyDescent="0.25">
-      <c r="B9" s="39"/>
-      <c r="C9" s="33"/>
+      <c r="B9" s="41"/>
+      <c r="C9" s="38"/>
       <c r="D9" s="3" t="s">
         <v>37</v>
       </c>
@@ -1224,14 +1239,16 @@
       <c r="H9" s="16" t="s">
         <v>54</v>
       </c>
-      <c r="I9" s="40" t="s">
+      <c r="I9" s="32" t="s">
         <v>59</v>
       </c>
-      <c r="J9" s="26"/>
+      <c r="J9" s="44" t="s">
+        <v>76</v>
+      </c>
     </row>
     <row r="10" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B10" s="39"/>
-      <c r="C10" s="33"/>
+      <c r="B10" s="41"/>
+      <c r="C10" s="38"/>
       <c r="D10" s="3" t="s">
         <v>11</v>
       </c>
@@ -1255,8 +1272,8 @@
       </c>
     </row>
     <row r="11" spans="2:10" ht="30" x14ac:dyDescent="0.25">
-      <c r="B11" s="39"/>
-      <c r="C11" s="33"/>
+      <c r="B11" s="41"/>
+      <c r="C11" s="38"/>
       <c r="D11" s="3" t="s">
         <v>12</v>
       </c>
@@ -1278,8 +1295,8 @@
       <c r="J11" s="26"/>
     </row>
     <row r="12" spans="2:10" ht="60" x14ac:dyDescent="0.25">
-      <c r="B12" s="39"/>
-      <c r="C12" s="33"/>
+      <c r="B12" s="41"/>
+      <c r="C12" s="38"/>
       <c r="D12" s="3" t="s">
         <v>29</v>
       </c>
@@ -1301,8 +1318,8 @@
       <c r="J12" s="26"/>
     </row>
     <row r="13" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B13" s="39"/>
-      <c r="C13" s="33"/>
+      <c r="B13" s="41"/>
+      <c r="C13" s="38"/>
       <c r="D13" s="3" t="s">
         <v>39</v>
       </c>
@@ -1324,8 +1341,8 @@
       <c r="J13" s="26"/>
     </row>
     <row r="14" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B14" s="39"/>
-      <c r="C14" s="33"/>
+      <c r="B14" s="41"/>
+      <c r="C14" s="38"/>
       <c r="D14" s="3" t="s">
         <v>13</v>
       </c>
@@ -1347,7 +1364,7 @@
       <c r="J14" s="26"/>
     </row>
     <row r="15" spans="2:10" ht="30" x14ac:dyDescent="0.25">
-      <c r="B15" s="35"/>
+      <c r="B15" s="42"/>
       <c r="C15" s="21" t="s">
         <v>66</v>
       </c>
@@ -1372,10 +1389,10 @@
       <c r="J15" s="26"/>
     </row>
     <row r="16" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B16" s="34" t="s">
+      <c r="B16" s="36" t="s">
         <v>25</v>
       </c>
-      <c r="C16" s="33" t="s">
+      <c r="C16" s="38" t="s">
         <v>26</v>
       </c>
       <c r="D16" s="3" t="s">
@@ -1397,8 +1414,8 @@
       <c r="J16" s="26"/>
     </row>
     <row r="17" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B17" s="34"/>
-      <c r="C17" s="33"/>
+      <c r="B17" s="36"/>
+      <c r="C17" s="38"/>
       <c r="D17" s="3" t="s">
         <v>33</v>
       </c>
@@ -1418,10 +1435,10 @@
       <c r="J17" s="26"/>
     </row>
     <row r="18" spans="2:10" ht="30" x14ac:dyDescent="0.25">
-      <c r="B18" s="34" t="s">
+      <c r="B18" s="36" t="s">
         <v>42</v>
       </c>
-      <c r="C18" s="33" t="s">
+      <c r="C18" s="38" t="s">
         <v>44</v>
       </c>
       <c r="D18" s="3" t="s">
@@ -1443,8 +1460,8 @@
       <c r="J18" s="26"/>
     </row>
     <row r="19" spans="2:10" ht="30" x14ac:dyDescent="0.25">
-      <c r="B19" s="34"/>
-      <c r="C19" s="33"/>
+      <c r="B19" s="36"/>
+      <c r="C19" s="38"/>
       <c r="D19" s="3" t="s">
         <v>47</v>
       </c>
@@ -1466,8 +1483,8 @@
       <c r="J19" s="26"/>
     </row>
     <row r="20" spans="2:10" ht="30" x14ac:dyDescent="0.25">
-      <c r="B20" s="34"/>
-      <c r="C20" s="33"/>
+      <c r="B20" s="36"/>
+      <c r="C20" s="38"/>
       <c r="D20" s="3" t="s">
         <v>50</v>
       </c>
@@ -1487,8 +1504,8 @@
       <c r="J20" s="26"/>
     </row>
     <row r="21" spans="2:10" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B21" s="36"/>
-      <c r="C21" s="37"/>
+      <c r="B21" s="37"/>
+      <c r="C21" s="39"/>
       <c r="D21" s="11" t="s">
         <v>64</v>
       </c>
@@ -1508,11 +1525,11 @@
       </c>
     </row>
     <row r="23" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="C23" s="42"/>
-      <c r="D23" s="43" t="s">
+      <c r="C23" s="34"/>
+      <c r="D23" s="35" t="s">
         <v>71</v>
       </c>
-      <c r="E23" s="42" t="s">
+      <c r="E23" s="34" t="s">
         <v>70</v>
       </c>
     </row>
@@ -1524,20 +1541,20 @@
         <f>COUNTIF($I$3:$I$21,C24)</f>
         <v>11</v>
       </c>
-      <c r="E24" s="41">
+      <c r="E24" s="33">
         <f>D24/SUM($D$24:$D$27)</f>
         <v>0.57894736842105265</v>
       </c>
     </row>
     <row r="25" spans="2:10" ht="30" x14ac:dyDescent="0.25">
-      <c r="C25" s="40" t="s">
+      <c r="C25" s="32" t="s">
         <v>59</v>
       </c>
       <c r="D25" s="29">
         <f t="shared" ref="D25:D27" si="0">COUNTIF($I$3:$I$21,C25)</f>
         <v>4</v>
       </c>
-      <c r="E25" s="41">
+      <c r="E25" s="33">
         <f t="shared" ref="E25:E27" si="1">D25/SUM($D$24:$D$27)</f>
         <v>0.21052631578947367</v>
       </c>
@@ -1550,7 +1567,7 @@
         <f t="shared" si="0"/>
         <v>4</v>
       </c>
-      <c r="E26" s="41">
+      <c r="E26" s="33">
         <f t="shared" si="1"/>
         <v>0.21052631578947367</v>
       </c>
@@ -1563,7 +1580,7 @@
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="E27" s="41">
+      <c r="E27" s="33">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>

</xml_diff>

<commit_message>
update status for rs485
</commit_message>
<xml_diff>
--- a/References/Modules.xlsx
+++ b/References/Modules.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21001"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DBC5CD49-8A72-48A9-9B8E-44E137C7FF80}" xr6:coauthVersionLast="38" xr6:coauthVersionMax="38" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B6FE5B8B-100B-49E0-83AC-2A4033626EC4}" xr6:coauthVersionLast="38" xr6:coauthVersionMax="38" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="575" uniqueCount="77">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="460" uniqueCount="77">
   <si>
     <t>Hardware</t>
   </si>
@@ -265,7 +265,7 @@
     <t>Chưa đổ lên board test</t>
   </si>
   <si>
-    <t>thiếu bên slave</t>
+    <t xml:space="preserve">chưa test trên board </t>
   </si>
 </sst>
 </file>
@@ -714,6 +714,9 @@
     <xf numFmtId="0" fontId="0" fillId="8" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="14" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -738,10 +741,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="14" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="14" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
   </cellXfs>
@@ -1033,7 +1033,7 @@
   <dimension ref="B1:J27"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="B4" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="J6" sqref="J6"/>
+      <selection activeCell="K11" sqref="K11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1080,10 +1080,10 @@
       </c>
     </row>
     <row r="3" spans="2:10" ht="90" x14ac:dyDescent="0.25">
-      <c r="B3" s="42" t="s">
+      <c r="B3" s="43" t="s">
         <v>0</v>
       </c>
-      <c r="C3" s="43" t="s">
+      <c r="C3" s="44" t="s">
         <v>7</v>
       </c>
       <c r="D3" s="6" t="s">
@@ -1103,8 +1103,8 @@
       <c r="J3" s="25"/>
     </row>
     <row r="4" spans="2:10" ht="30" x14ac:dyDescent="0.25">
-      <c r="B4" s="36"/>
-      <c r="C4" s="38"/>
+      <c r="B4" s="37"/>
+      <c r="C4" s="39"/>
       <c r="D4" s="3" t="s">
         <v>2</v>
       </c>
@@ -1124,8 +1124,8 @@
       </c>
     </row>
     <row r="5" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B5" s="36"/>
-      <c r="C5" s="38" t="s">
+      <c r="B5" s="37"/>
+      <c r="C5" s="39" t="s">
         <v>3</v>
       </c>
       <c r="D5" s="3" t="s">
@@ -1147,8 +1147,8 @@
       </c>
     </row>
     <row r="6" spans="2:10" ht="30" x14ac:dyDescent="0.25">
-      <c r="B6" s="36"/>
-      <c r="C6" s="38"/>
+      <c r="B6" s="37"/>
+      <c r="C6" s="39"/>
       <c r="D6" s="3" t="s">
         <v>8</v>
       </c>
@@ -1165,13 +1165,13 @@
       <c r="I6" s="28" t="s">
         <v>58</v>
       </c>
-      <c r="J6" s="45" t="s">
+      <c r="J6" s="36" t="s">
         <v>73</v>
       </c>
     </row>
     <row r="7" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B7" s="36"/>
-      <c r="C7" s="38"/>
+      <c r="B7" s="37"/>
+      <c r="C7" s="39"/>
       <c r="D7" s="3" t="s">
         <v>41</v>
       </c>
@@ -1193,10 +1193,10 @@
       </c>
     </row>
     <row r="8" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B8" s="40" t="s">
+      <c r="B8" s="41" t="s">
         <v>36</v>
       </c>
-      <c r="C8" s="38" t="s">
+      <c r="C8" s="39" t="s">
         <v>3</v>
       </c>
       <c r="D8" s="3" t="s">
@@ -1222,8 +1222,8 @@
       </c>
     </row>
     <row r="9" spans="2:10" ht="30" x14ac:dyDescent="0.25">
-      <c r="B9" s="41"/>
-      <c r="C9" s="38"/>
+      <c r="B9" s="42"/>
+      <c r="C9" s="39"/>
       <c r="D9" s="3" t="s">
         <v>37</v>
       </c>
@@ -1240,15 +1240,15 @@
         <v>54</v>
       </c>
       <c r="I9" s="32" t="s">
-        <v>59</v>
-      </c>
-      <c r="J9" s="44" t="s">
+        <v>58</v>
+      </c>
+      <c r="J9" s="45" t="s">
         <v>76</v>
       </c>
     </row>
     <row r="10" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B10" s="41"/>
-      <c r="C10" s="38"/>
+      <c r="B10" s="42"/>
+      <c r="C10" s="39"/>
       <c r="D10" s="3" t="s">
         <v>11</v>
       </c>
@@ -1272,8 +1272,8 @@
       </c>
     </row>
     <row r="11" spans="2:10" ht="30" x14ac:dyDescent="0.25">
-      <c r="B11" s="41"/>
-      <c r="C11" s="38"/>
+      <c r="B11" s="42"/>
+      <c r="C11" s="39"/>
       <c r="D11" s="3" t="s">
         <v>12</v>
       </c>
@@ -1295,8 +1295,8 @@
       <c r="J11" s="26"/>
     </row>
     <row r="12" spans="2:10" ht="60" x14ac:dyDescent="0.25">
-      <c r="B12" s="41"/>
-      <c r="C12" s="38"/>
+      <c r="B12" s="42"/>
+      <c r="C12" s="39"/>
       <c r="D12" s="3" t="s">
         <v>29</v>
       </c>
@@ -1318,8 +1318,8 @@
       <c r="J12" s="26"/>
     </row>
     <row r="13" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B13" s="41"/>
-      <c r="C13" s="38"/>
+      <c r="B13" s="42"/>
+      <c r="C13" s="39"/>
       <c r="D13" s="3" t="s">
         <v>39</v>
       </c>
@@ -1341,8 +1341,8 @@
       <c r="J13" s="26"/>
     </row>
     <row r="14" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B14" s="41"/>
-      <c r="C14" s="38"/>
+      <c r="B14" s="42"/>
+      <c r="C14" s="39"/>
       <c r="D14" s="3" t="s">
         <v>13</v>
       </c>
@@ -1364,7 +1364,7 @@
       <c r="J14" s="26"/>
     </row>
     <row r="15" spans="2:10" ht="30" x14ac:dyDescent="0.25">
-      <c r="B15" s="42"/>
+      <c r="B15" s="43"/>
       <c r="C15" s="21" t="s">
         <v>66</v>
       </c>
@@ -1389,10 +1389,10 @@
       <c r="J15" s="26"/>
     </row>
     <row r="16" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B16" s="36" t="s">
+      <c r="B16" s="37" t="s">
         <v>25</v>
       </c>
-      <c r="C16" s="38" t="s">
+      <c r="C16" s="39" t="s">
         <v>26</v>
       </c>
       <c r="D16" s="3" t="s">
@@ -1414,8 +1414,8 @@
       <c r="J16" s="26"/>
     </row>
     <row r="17" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B17" s="36"/>
-      <c r="C17" s="38"/>
+      <c r="B17" s="37"/>
+      <c r="C17" s="39"/>
       <c r="D17" s="3" t="s">
         <v>33</v>
       </c>
@@ -1435,10 +1435,10 @@
       <c r="J17" s="26"/>
     </row>
     <row r="18" spans="2:10" ht="30" x14ac:dyDescent="0.25">
-      <c r="B18" s="36" t="s">
+      <c r="B18" s="37" t="s">
         <v>42</v>
       </c>
-      <c r="C18" s="38" t="s">
+      <c r="C18" s="39" t="s">
         <v>44</v>
       </c>
       <c r="D18" s="3" t="s">
@@ -1460,8 +1460,8 @@
       <c r="J18" s="26"/>
     </row>
     <row r="19" spans="2:10" ht="30" x14ac:dyDescent="0.25">
-      <c r="B19" s="36"/>
-      <c r="C19" s="38"/>
+      <c r="B19" s="37"/>
+      <c r="C19" s="39"/>
       <c r="D19" s="3" t="s">
         <v>47</v>
       </c>
@@ -1483,8 +1483,8 @@
       <c r="J19" s="26"/>
     </row>
     <row r="20" spans="2:10" ht="30" x14ac:dyDescent="0.25">
-      <c r="B20" s="36"/>
-      <c r="C20" s="38"/>
+      <c r="B20" s="37"/>
+      <c r="C20" s="39"/>
       <c r="D20" s="3" t="s">
         <v>50</v>
       </c>
@@ -1504,8 +1504,8 @@
       <c r="J20" s="26"/>
     </row>
     <row r="21" spans="2:10" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B21" s="37"/>
-      <c r="C21" s="39"/>
+      <c r="B21" s="38"/>
+      <c r="C21" s="40"/>
       <c r="D21" s="11" t="s">
         <v>64</v>
       </c>
@@ -1552,11 +1552,11 @@
       </c>
       <c r="D25" s="29">
         <f t="shared" ref="D25:D27" si="0">COUNTIF($I$3:$I$21,C25)</f>
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="E25" s="33">
         <f t="shared" ref="E25:E27" si="1">D25/SUM($D$24:$D$27)</f>
-        <v>0.21052631578947367</v>
+        <v>0.15789473684210525</v>
       </c>
     </row>
     <row r="26" spans="2:10" x14ac:dyDescent="0.25">
@@ -1565,11 +1565,11 @@
       </c>
       <c r="D26" s="29">
         <f t="shared" si="0"/>
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="E26" s="33">
         <f t="shared" si="1"/>
-        <v>0.21052631578947367</v>
+        <v>0.26315789473684209</v>
       </c>
     </row>
     <row r="27" spans="2:10" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
update status for serial debug
</commit_message>
<xml_diff>
--- a/References/Modules.xlsx
+++ b/References/Modules.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21001"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B6FE5B8B-100B-49E0-83AC-2A4033626EC4}" xr6:coauthVersionLast="38" xr6:coauthVersionMax="38" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{45F71BC4-EAE0-4E19-8540-7EA86A00F45C}" xr6:coauthVersionLast="38" xr6:coauthVersionMax="38" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="460" uniqueCount="77">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="116" uniqueCount="78">
   <si>
     <t>Hardware</t>
   </si>
@@ -259,13 +259,17 @@
     <t>Chưa mượn thầy</t>
   </si>
   <si>
-    <t>Chưa đổ lên board để test</t>
-  </si>
-  <si>
     <t>Chưa đổ lên board test</t>
   </si>
   <si>
     <t xml:space="preserve">chưa test trên board </t>
+  </si>
+  <si>
+    <t>Chưa đổ lên board để test
+chưa đưa qua master device</t>
+  </si>
+  <si>
+    <t>Chưa chuyển qua slave</t>
   </si>
 </sst>
 </file>
@@ -352,7 +356,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="19">
+  <borders count="20">
     <border>
       <left/>
       <right/>
@@ -604,6 +608,15 @@
       <right style="medium">
         <color indexed="64"/>
       </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
       <top/>
       <bottom/>
       <diagonal/>
@@ -613,7 +626,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="9" fontId="2" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="46">
+  <cellXfs count="48">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -698,9 +711,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="7" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -717,32 +727,41 @@
     <xf numFmtId="0" fontId="0" fillId="9" borderId="14" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="14" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="19" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="19" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -1032,20 +1051,21 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="B1:J27"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B4" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="K11" sqref="K11"/>
+    <sheetView tabSelected="1" topLeftCell="B19" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="J27" sqref="J27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="4.5703125" customWidth="1"/>
-    <col min="2" max="3" width="9.5703125" style="1" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="9.5703125" style="1" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="10.140625" style="1" customWidth="1"/>
     <col min="4" max="4" width="17.5703125" style="4" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="41" style="5" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="37" style="5" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="6.28515625" style="7" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="9.140625" customWidth="1"/>
-    <col min="9" max="9" width="10.7109375" style="4" customWidth="1"/>
+    <col min="9" max="9" width="12" style="4" customWidth="1"/>
     <col min="10" max="10" width="36.85546875" style="24" customWidth="1"/>
   </cols>
   <sheetData>
@@ -1097,7 +1117,7 @@
         <v>1</v>
       </c>
       <c r="H3" s="20"/>
-      <c r="I3" s="32" t="s">
+      <c r="I3" s="31" t="s">
         <v>59</v>
       </c>
       <c r="J3" s="25"/>
@@ -1116,7 +1136,7 @@
         <v>1</v>
       </c>
       <c r="H4" s="16"/>
-      <c r="I4" s="32" t="s">
+      <c r="I4" s="31" t="s">
         <v>59</v>
       </c>
       <c r="J4" s="26" t="s">
@@ -1165,7 +1185,7 @@
       <c r="I6" s="28" t="s">
         <v>58</v>
       </c>
-      <c r="J6" s="36" t="s">
+      <c r="J6" s="35" t="s">
         <v>73</v>
       </c>
     </row>
@@ -1185,14 +1205,14 @@
         <v>1</v>
       </c>
       <c r="H7" s="16"/>
-      <c r="I7" s="32" t="s">
+      <c r="I7" s="31" t="s">
         <v>59</v>
       </c>
       <c r="J7" s="26" t="s">
         <v>61</v>
       </c>
     </row>
-    <row r="8" spans="2:10" x14ac:dyDescent="0.25">
+    <row r="8" spans="2:10" ht="30" x14ac:dyDescent="0.25">
       <c r="B8" s="41" t="s">
         <v>36</v>
       </c>
@@ -1214,11 +1234,11 @@
       <c r="H8" s="16" t="s">
         <v>54</v>
       </c>
-      <c r="I8" s="28" t="s">
-        <v>58</v>
-      </c>
-      <c r="J8" s="26" t="s">
-        <v>74</v>
+      <c r="I8" s="31" t="s">
+        <v>59</v>
+      </c>
+      <c r="J8" s="45" t="s">
+        <v>76</v>
       </c>
     </row>
     <row r="9" spans="2:10" ht="30" x14ac:dyDescent="0.25">
@@ -1239,11 +1259,11 @@
       <c r="H9" s="16" t="s">
         <v>54</v>
       </c>
-      <c r="I9" s="32" t="s">
+      <c r="I9" s="28" t="s">
         <v>58</v>
       </c>
-      <c r="J9" s="45" t="s">
-        <v>76</v>
+      <c r="J9" s="36" t="s">
+        <v>75</v>
       </c>
     </row>
     <row r="10" spans="2:10" x14ac:dyDescent="0.25">
@@ -1268,7 +1288,7 @@
         <v>58</v>
       </c>
       <c r="J10" s="26" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
     </row>
     <row r="11" spans="2:10" ht="30" x14ac:dyDescent="0.25">
@@ -1383,10 +1403,12 @@
       <c r="H15" s="16" t="s">
         <v>54</v>
       </c>
-      <c r="I15" s="29" t="s">
-        <v>57</v>
-      </c>
-      <c r="J15" s="26"/>
+      <c r="I15" s="31" t="s">
+        <v>59</v>
+      </c>
+      <c r="J15" s="45" t="s">
+        <v>77</v>
+      </c>
     </row>
     <row r="16" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B16" s="37" t="s">
@@ -1514,22 +1536,22 @@
       </c>
       <c r="F21" s="12"/>
       <c r="G21" s="18"/>
-      <c r="H21" s="31" t="s">
+      <c r="H21" s="30" t="s">
         <v>55</v>
       </c>
-      <c r="I21" s="30" t="s">
-        <v>57</v>
+      <c r="I21" s="31" t="s">
+        <v>59</v>
       </c>
       <c r="J21" s="23" t="s">
         <v>63</v>
       </c>
     </row>
     <row r="23" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="C23" s="34"/>
-      <c r="D23" s="35" t="s">
+      <c r="C23" s="33"/>
+      <c r="D23" s="34" t="s">
         <v>71</v>
       </c>
-      <c r="E23" s="34" t="s">
+      <c r="E23" s="33" t="s">
         <v>70</v>
       </c>
     </row>
@@ -1539,24 +1561,28 @@
       </c>
       <c r="D24" s="29">
         <f>COUNTIF($I$3:$I$21,C24)</f>
-        <v>11</v>
-      </c>
-      <c r="E24" s="33">
+        <v>9</v>
+      </c>
+      <c r="E24" s="32">
         <f>D24/SUM($D$24:$D$27)</f>
-        <v>0.57894736842105265</v>
-      </c>
-    </row>
-    <row r="25" spans="2:10" ht="30" x14ac:dyDescent="0.25">
-      <c r="C25" s="32" t="s">
+        <v>0.47368421052631576</v>
+      </c>
+    </row>
+    <row r="25" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="C25" s="31" t="s">
         <v>59</v>
       </c>
       <c r="D25" s="29">
         <f t="shared" ref="D25:D27" si="0">COUNTIF($I$3:$I$21,C25)</f>
-        <v>3</v>
-      </c>
-      <c r="E25" s="33">
+        <v>6</v>
+      </c>
+      <c r="E25" s="32">
         <f t="shared" ref="E25:E27" si="1">D25/SUM($D$24:$D$27)</f>
-        <v>0.15789473684210525</v>
+        <v>0.31578947368421051</v>
+      </c>
+      <c r="F25" s="47">
+        <f>E25+E26</f>
+        <v>0.52631578947368418</v>
       </c>
     </row>
     <row r="26" spans="2:10" x14ac:dyDescent="0.25">
@@ -1565,12 +1591,13 @@
       </c>
       <c r="D26" s="29">
         <f t="shared" si="0"/>
-        <v>5</v>
-      </c>
-      <c r="E26" s="33">
+        <v>4</v>
+      </c>
+      <c r="E26" s="32">
         <f t="shared" si="1"/>
-        <v>0.26315789473684209</v>
-      </c>
+        <v>0.21052631578947367</v>
+      </c>
+      <c r="F26" s="46"/>
     </row>
     <row r="27" spans="2:10" x14ac:dyDescent="0.25">
       <c r="C27" s="27" t="s">
@@ -1580,13 +1607,14 @@
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="E27" s="33">
+      <c r="E27" s="32">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
     </row>
   </sheetData>
-  <mergeCells count="9">
+  <mergeCells count="10">
+    <mergeCell ref="F25:F26"/>
     <mergeCell ref="B18:B21"/>
     <mergeCell ref="C18:C21"/>
     <mergeCell ref="B8:B15"/>
@@ -1598,7 +1626,7 @@
     <mergeCell ref="C5:C7"/>
   </mergeCells>
   <dataValidations count="1">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="I3:I21 C25:C26" xr:uid="{F40B1D61-2730-4EB1-9419-B31D0F64C450}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C25:C26 I3:I21" xr:uid="{F40B1D61-2730-4EB1-9419-B31D0F64C450}">
       <formula1>"Not start,In process,Review,Done"</formula1>
     </dataValidation>
   </dataValidations>

</xml_diff>